<commit_message>
changed title of BOM
</commit_message>
<xml_diff>
--- a/sonar/preprocessor_v3/design_blocks/filter/BOM.xlsx
+++ b/sonar/preprocessor_v3/design_blocks/filter/BOM.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kraem\ARVP\au_hardware\sonar\preprocessor_v3\design_blocks\filter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\ARVP\Repository\au_hardware\sonar\preprocessor_v3\design_blocks\filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,9 +83,6 @@
     <t>350k Ohm</t>
   </si>
   <si>
-    <t>Torpedo Board V3: Bill of Materials</t>
-  </si>
-  <si>
     <t>Shematic Reference Number</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>*not available from Digikey in single quantities</t>
+  </si>
+  <si>
+    <t>Filter Prototype: Bill of Materials</t>
   </si>
 </sst>
 </file>
@@ -374,6 +374,8 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,8 +385,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -703,42 +703,42 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -755,13 +755,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="1">
         <v>23.33</v>
@@ -774,7 +774,7 @@
         <v>23.33</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -784,11 +784,11 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E4" s="1">
         <v>1.31</v>
@@ -797,22 +797,22 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G22" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G21" si="0">E4*F4</f>
         <v>1.31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>37</v>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1">
         <v>0.5</v>
@@ -832,11 +832,11 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>52</v>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <v>0.56999999999999995</v>
@@ -856,11 +856,11 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="E7" s="1">
         <v>0.2</v>
@@ -880,13 +880,13 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="F8" s="1">
@@ -904,11 +904,11 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>0.14000000000000001</v>
@@ -928,8 +928,8 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
@@ -952,8 +952,8 @@
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>60</v>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>61</v>
+      <c r="C12" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -995,16 +995,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>62</v>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1">
         <v>0.14000000000000001</v>
@@ -1019,13 +1019,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>63</v>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -1043,13 +1043,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>64</v>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
+      <c r="C16" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
@@ -1091,13 +1091,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>66</v>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
@@ -1115,16 +1115,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E18" s="1">
         <v>0.15</v>
@@ -1139,16 +1139,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="1">
         <v>0.13</v>
@@ -1163,16 +1163,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E20" s="1">
         <v>0.13</v>
@@ -1187,16 +1187,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E21" s="1">
         <v>0.2</v>
@@ -1211,25 +1211,25 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1">
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>